<commit_message>
Writing Output into the Excel File
</commit_message>
<xml_diff>
--- a/Max Pipeline Adjustments/Pipeline/Prompts.xlsx
+++ b/Max Pipeline Adjustments/Pipeline/Prompts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,11 @@
           <t>fn_abstracts</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Output</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -593,28 +598,33 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="R2" t="n">
-        <v>0.2205128205128205</v>
+        <v>0.1255144032921811</v>
       </c>
       <c r="S2" t="n">
-        <v>0.03184713375796178</v>
+        <v>0.02073732718894009</v>
       </c>
       <c r="T2" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.9838709677419355</v>
       </c>
       <c r="U2" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="V2" t="n">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="W2" t="n">
-        <v>152</v>
+        <v>425</v>
       </c>
       <c r="X2" t="n">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>[['36823236', '35841079', '21608000', '25024623', '21900788'], ['35309311', '32071558', '28620221', '34843069', '37328872'], ['35858897', '36183106', '36698192', '35395830', '35278227'], ['35099348', '37918086'], ['29104502', '35505419', '37539053', '34882906', '37337578'], ['37498509', '36812711', '36998425', '36049782', '26420953'], ['37864199', '36983624'], ['27601441', '29303079', '32077830'], ['36544529', '37283714', '27176654', '36423545', '35902883'], ['36462157', '38164852', '25320545'], ['26691057', '30854976', '37282819'], ['26934883', '37329808', '37494836'], ['37798761', '28627746', '37114594', '35100287', '37852157'], ['24036368', '32827326', '33317249', '37626924', '27539153'], ['32928296', '37604091', '36029414', '37079286', '35563807'], ['38442726', '35932064', '27819130', '37271943', '32775366'], ["36093813' , '37365036", '24415865'], ['31281379', '31591328'], ['37874430', '35484432', '32621283', '32267915'], ['27481213', '27495745', '22228987'], ['33554346', '34565478', '37167639'], ['30394698', '35659360', '30885249'], ['28297787', '35440002', '38013053', '27153445', '36552767'], ['31520775', '19642968', '19941447', '24157970', '20220785'], ['30106103', '30019838', '30248223', '27591095', "27468195' ,"], ['32880852', '31755595', '32962510'], ['38419761', '24457953', '31435712', '35883205', '36330597'], ['37345718', '32633558', '34186042', '37226279', '37742014'], ['31048740', '35084178', '28805262', '37084952'], ['25450712', '33143043', '31781620', '29497038', '32865681'], ['30375438', '35578365', '31592593'], ['36703021', '37298538', '37507381', '38105754', '38198960'], ['35199612', '37501214', '38159943'], ['37980535', '30635047', '32816183', '33935044', '35006577'], ['30223894', '23531302', '21200380', '22678013', '27500218'], ['37787035', '35036058', '30834983', '34518510', '33384547'], ['25613158', '32506351', '35293541', '26811102'], ['33293768', '34046793', '33145022', '31760709', '34012193'], ['25006200', '31147180', '36649501', '25722117', '28583205'], ['30048056', '33389680', '22533821', '34809720', '30675167'], ['23686136', '26464632', '22753359', '31245923', '37226801'], ['36359733', '36735212', '36411771', '36183364', '27908750'], ['33555212', '33348053', '30850965', '33060633', '33785758'], ['35435145', '34775285', '32374186', '26310071'], ['29266258', '22416179', '29286155', '23002959', '36674693'], ['33708992', '33342075', '42774189'], ['35075209', '38402155', '32389821', '33617844', '34016164'], ['19780871', '26369870', '33349209', '27805290', '30538216'], ['20943307', '24507685', '36941658', '32011099', '38356602'], ['32245503', '29861737', '30901579', '35186473'], ['32535098', '30810620', '37031397', '36610716', '25315017'], ['26876222', '33629329', '22182291', '30635054', '25445161'], ['27365486', '28382720', '37899504', '31452434', '34859376'], ['28494546', '35831878', '37133409', '30402110', '34174353'], ['24488807', '35315848', '37064607', '30700543', '33855751'], ['17869217', '26157751', '28544786', '23809154', '19684854'], ['34343826', '31508820', '17543295', '27981544', '28115038'], ['33078915', '27876093', '29130552', '34158112', '31768225'], ['32546282', '33855079', '24835895', '19686763'], ['27430962', '21289474', '30114694', '29145157', '34689832'], ['18176050', '32289375', '22609227', '29362496', '29264872'], ['24104560', '29150810', '34514810', '31550244', '25490388'], ['32357508', '34627378', '20178458', '22735033', '34712665'], ['19398237', '29398486', '21966929', '34256837', '28301671'], ['29512750', '28217916', '27028843', '26353075', '34416908'], ['29666468', '21326862', '25678175'], ['22927965', '33246509', '20367252', '23402186', '26861623'], ['20096523', '16469408', '32650827', '29290652'], ['19422480', '27280796', '29804359', '32801431', '31525863'], ['32867602', '25426285', '29223366', '38016185', '18486597'], ['28413861', '32603821', '16150456', '31552493', '30979485'], ['27960154', '24481983', '22320928', '31551525', '27543493'], ['28610623', '22167104', '31952158', '23855301', '27956229'], ['16233854', '23807535', '28585911', '38540717', '38413394'], ['24886681', '21356258', '22432472', '26125913', '32503644'], ['20025519', '29187911', '21537835', '25501583', '37964155'], ['27130910', '26389810', '19559033', '20824962', '26877613'], ['29110545', '30230766', '25473446', '25639333', '31982488'], ['14568247', '29293276', '23150236', '23782511', '22941276'], ['26153152', '18522880', '20663626', '25842730', '21810549'], ['25145391', '26643997', '38360740', '21770423', '22056375'], ['19399744', '37997442', '38474368', '28782844', '38160190'], ['34865351', '23638052', '19455046', '19056764', '24144538'], ['27938474', '19242797', '30453717', '19476212', '29074333'], ['25063290', '24115681', '38429940', '28035356', '24682874'], ['21239501', '33238629', '24967970', '17903050'], ['26194009', '24942592', '26839564', '28625529'], ['21145826', '20184502', '25268050', '26358689'], ['23849977', '20182823', '30631870', '21989829'], ['24815159', '26155209', '26599535', '25446803', '21269936'], ['24116127', '27878730', '21391433', '17903371', '17952094'], ['26983390', '24417995', '25890163', '28073411', '25654284'], ['25203804', '25518471', '15850515', '16108363', '38474048'], ['26540984'], ['23522251', '15650781', '24748190'], ['21526984', '30461638', '27339398'], ['29285145', '23980370', '31885614', '27405780', '34715410'], ['35721175', '34504910', '27785340', '34711695'], ['21516840', '37576406', '29844633'], ['34796180']]</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -662,6 +672,7 @@
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -708,6 +719,7 @@
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -754,6 +766,7 @@
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>